<commit_message>
Only keep the last model
</commit_message>
<xml_diff>
--- a/4-Extend.xlsx
+++ b/4-Extend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks_000\Desktop\Mentorship\!GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8833BBD-027A-46BD-89D8-18C5C746FD36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6EDD2E-7503-4015-BB7E-D09B987CAAF4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21804" windowHeight="8796" xr2:uid="{FA779093-122C-4A05-86C7-F98EA3A699EC}"/>
   </bookViews>
@@ -1612,7 +1612,7 @@
   <dimension ref="A1:AJ26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Nice labels and order by variance
</commit_message>
<xml_diff>
--- a/4-Extend.xlsx
+++ b/4-Extend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks_000\Desktop\Mentorship\!GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E34C0E-D3EA-4A4C-9ACF-C2F17AA5CAAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1E2C88-BFEF-456B-8CE9-2757654CD697}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1212" yWindow="0" windowWidth="21828" windowHeight="12384" xr2:uid="{FA779093-122C-4A05-86C7-F98EA3A699EC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="61">
   <si>
     <t>Scenario</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>SSC: parameters (rho) + implementation</t>
+  </si>
+  <si>
+    <t>Dynamic stopping</t>
+  </si>
+  <si>
+    <t>Increased model size</t>
+  </si>
+  <si>
+    <t>Narrow more aggressively</t>
   </si>
 </sst>
 </file>
@@ -1597,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879D3BE8-5908-4BE5-BD92-5B34615E80E7}">
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="K5" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2968,7 +2977,9 @@
         <f t="shared" si="19"/>
         <v>14263.701367331501</v>
       </c>
-      <c r="X21" s="33"/>
+      <c r="X21" s="33">
+        <v>0.25955408552301701</v>
+      </c>
       <c r="Y21" s="32">
         <v>7.8434654010144603E-3</v>
       </c>
@@ -3163,16 +3174,26 @@
         <v>72.549880042480254</v>
       </c>
       <c r="X23" s="7"/>
-      <c r="Y23" s="25"/>
+      <c r="Y23">
+        <v>2.2960116233104198E-2</v>
+      </c>
       <c r="Z23" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AA23" s="42"/>
+      <c r="AA23" s="70">
+        <v>8.7593013078191206E-6</v>
+      </c>
       <c r="AB23" s="25" t="s">
         <v>19</v>
       </c>
+      <c r="AC23">
+        <v>4.0139396740152197E-3</v>
+      </c>
       <c r="AD23" t="s">
         <v>19</v>
+      </c>
+      <c r="AE23">
+        <v>2.7430071377510501</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.3">
@@ -3469,6 +3490,21 @@
         <v>57</v>
       </c>
     </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B10:F10"/>
@@ -3477,6 +3513,18 @@
     <mergeCell ref="X10:AE10"/>
   </mergeCells>
   <conditionalFormatting sqref="X12:X16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X17:X21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
More rigorous re-evaluations Re-evaluated on seeds 100-129 instead of 0-4
</commit_message>
<xml_diff>
--- a/4-Extend.xlsx
+++ b/4-Extend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks_000\Desktop\Mentorship\!GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9D0BAE-D4CD-4CBA-9A5C-18E20D662882}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCE30A1-8E0B-4E13-85A4-4968AD4EE277}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1212" yWindow="0" windowWidth="21828" windowHeight="12384" xr2:uid="{FA779093-122C-4A05-86C7-F98EA3A699EC}"/>
   </bookViews>
@@ -195,9 +195,6 @@
     <t>re_seeds</t>
   </si>
   <si>
-    <t>0 - 5</t>
-  </si>
-  <si>
     <t>SSC: parameters (rho) + implementation</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>sp_minimize</t>
+  </si>
+  <si>
+    <t>[100, 130)</t>
   </si>
 </sst>
 </file>
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879D3BE8-5908-4BE5-BD92-5B34615E80E7}">
   <dimension ref="A1:AE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="H2" s="43" t="s">
         <v>45</v>
@@ -2146,7 +2146,7 @@
         <v>10000</v>
       </c>
       <c r="X13" s="7">
-        <v>0.10918688740324201</v>
+        <v>0.13482600763470201</v>
       </c>
       <c r="Y13">
         <v>6.3720283621781096E-3</v>
@@ -2253,7 +2253,7 @@
         <v>10000</v>
       </c>
       <c r="X14" s="7">
-        <v>0.10433078398359601</v>
+        <v>0.12200828732853999</v>
       </c>
       <c r="Y14">
         <v>7.1515104499875201E-3</v>
@@ -2362,7 +2362,7 @@
         <v>10000</v>
       </c>
       <c r="X15" s="7">
-        <v>0.36385055029548702</v>
+        <v>0.375835493867756</v>
       </c>
       <c r="Y15">
         <v>1.9189713145768999E-3</v>
@@ -2471,7 +2471,7 @@
         <v>10000</v>
       </c>
       <c r="X16" s="33">
-        <v>0.34099523439767898</v>
+        <v>0.34684615824313197</v>
       </c>
       <c r="Y16" s="33">
         <v>1.2361374045736001E-3</v>
@@ -2671,7 +2671,7 @@
         <v>204.25784276515549</v>
       </c>
       <c r="X18" s="7">
-        <v>0.12670147474967</v>
+        <v>0.120615213788776</v>
       </c>
       <c r="Y18">
         <v>8.97835455410834E-3</v>
@@ -2778,7 +2778,7 @@
         <v>184.98574914007199</v>
       </c>
       <c r="X19" s="7">
-        <v>0.109416858664647</v>
+        <v>0.120191724473232</v>
       </c>
       <c r="Y19" s="25">
         <v>1.60776127264157E-2</v>
@@ -2887,7 +2887,7 @@
         <v>2285.9481156245301</v>
       </c>
       <c r="X20" s="7">
-        <v>0.35879076206579102</v>
+        <v>0.35035041030597203</v>
       </c>
       <c r="Y20" s="25">
         <v>6.0936401066759402E-4</v>
@@ -2996,7 +2996,7 @@
         <v>14263.701367331501</v>
       </c>
       <c r="X21" s="33">
-        <v>0.25955408552301701</v>
+        <v>0.26465531218853899</v>
       </c>
       <c r="Y21" s="32">
         <v>7.8434654010144603E-3</v>
@@ -3196,7 +3196,7 @@
         <v>72.549880042480254</v>
       </c>
       <c r="X23" s="7">
-        <v>0.130582679944476</v>
+        <v>0.129573706828434</v>
       </c>
       <c r="Y23">
         <v>5.8045218086709097E-3</v>
@@ -3303,7 +3303,7 @@
         <v>74.242985887545998</v>
       </c>
       <c r="X24" s="7">
-        <v>0.12651559086210301</v>
+        <v>0.12868836723166699</v>
       </c>
       <c r="Y24">
         <v>1.2072002534284101E-3</v>
@@ -3412,7 +3412,7 @@
         <v>563.29878202896998</v>
       </c>
       <c r="X25" s="7">
-        <v>0.465087850104628</v>
+        <v>0.46669992536550797</v>
       </c>
       <c r="Y25">
         <v>1.00264024608149E-3</v>
@@ -3521,7 +3521,7 @@
         <v>2740.7784473637498</v>
       </c>
       <c r="X26" s="7">
-        <v>0.15152497279535199</v>
+        <v>0.151549683075583</v>
       </c>
       <c r="Y26" s="13">
         <v>1.08193051300563E-2</v>
@@ -3562,37 +3562,37 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PCA effect on encoding
</commit_message>
<xml_diff>
--- a/4-Extend.xlsx
+++ b/4-Extend.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks_000\Desktop\Mentorship\!GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1D4D87-F3E3-4353-B795-9EE4D80336A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD77853D-6C2E-47DF-AC34-1F0D4B5346A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1212" yWindow="0" windowWidth="21828" windowHeight="12384" xr2:uid="{FA779093-122C-4A05-86C7-F98EA3A699EC}"/>
+    <workbookView xWindow="1212" yWindow="0" windowWidth="21828" windowHeight="12384" xr2:uid="{FA779093-122C-4A05-86C7-F98EA3A699EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="70">
   <si>
     <t>Scenario</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>!!! NO PCA</t>
+  </si>
+  <si>
+    <t>&lt;- [1.1056452  0.77839947 0.6102698  0.51495486 0.42832494 0.34158167], 0.30294085 1.3391844</t>
+  </si>
+  <si>
+    <t>vs [0.30793804 0.13396928 0.08810262 0.05079819 0.02864114 0.01859022], 0.016247319 0.5112661</t>
+  </si>
+  <si>
+    <t>0.7155123 -&gt; 0.92525244 vs 0.7304433</t>
   </si>
 </sst>
 </file>
@@ -1604,10 +1613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879D3BE8-5908-4BE5-BD92-5B34615E80E7}">
-  <dimension ref="A1:AE47"/>
+  <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3525,69 +3534,82 @@
         <v>58.397317625981898</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>66</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>